<commit_message>
update variables and tables
</commit_message>
<xml_diff>
--- a/final outputs for writing/Model results.xlsx
+++ b/final outputs for writing/Model results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="94">
   <si>
     <t>Females</t>
   </si>
@@ -145,6 +145,9 @@
     <t>BMI</t>
   </si>
   <si>
+    <t>&gt;0.9</t>
+  </si>
+  <si>
     <t>food_ran_out</t>
   </si>
   <si>
@@ -166,19 +169,7 @@
     <t>Covered</t>
   </si>
   <si>
-    <t>&gt;0.9</t>
-  </si>
-  <si>
     <t>home</t>
-  </si>
-  <si>
-    <t>Owned or being bought</t>
-  </si>
-  <si>
-    <t>Rented</t>
-  </si>
-  <si>
-    <t>Other Arrangement</t>
   </si>
   <si>
     <t>poverty_level_category</t>
@@ -196,16 +187,7 @@
     <t>emotional_support</t>
   </si>
   <si>
-    <t>SP doesn't need help</t>
-  </si>
-  <si>
     <t>health_care_access</t>
-  </si>
-  <si>
-    <t>There is no place</t>
-  </si>
-  <si>
-    <t>There is more than one place</t>
   </si>
   <si>
     <t>depression</t>
@@ -274,9 +256,6 @@
     <t>increased likelihood when renting when looking only at SDOH, but not significant when considering other variables.</t>
   </si>
   <si>
-    <t xml:space="preserve">increased likelihood when renting home. </t>
-  </si>
-  <si>
     <t>Increased likelihood as depression score increases.</t>
   </si>
   <si>
@@ -289,7 +268,7 @@
     <t>p-value = 0.7 and 0.2, so this is not significant.</t>
   </si>
   <si>
-    <t>Model</t>
+    <t>Names</t>
   </si>
   <si>
     <t>Nagelkerke</t>
@@ -416,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -483,6 +462,19 @@
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -945,7 +937,7 @@
         <v>0.026</v>
       </c>
       <c r="H7" s="7">
-        <v>3.47</v>
+        <v>3.43</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>11</v>
@@ -957,10 +949,10 @@
         <v>11</v>
       </c>
       <c r="L7" s="7">
-        <v>3.4</v>
+        <v>3.29</v>
       </c>
       <c r="M7" s="8">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -999,7 +991,7 @@
         <v>0.004</v>
       </c>
       <c r="H8" s="7">
-        <v>4.14</v>
+        <v>4.11</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>11</v>
@@ -1011,10 +1003,10 @@
         <v>11</v>
       </c>
       <c r="L8" s="7">
-        <v>3.57</v>
+        <v>3.47</v>
       </c>
       <c r="M8" s="8">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -1053,7 +1045,7 @@
         <v>0.004</v>
       </c>
       <c r="H9" s="7">
-        <v>5.45</v>
+        <v>5.27</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>11</v>
@@ -1065,10 +1057,10 @@
         <v>11</v>
       </c>
       <c r="L9" s="7">
-        <v>4.13</v>
+        <v>3.98</v>
       </c>
       <c r="M9" s="8">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -1107,7 +1099,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="7">
-        <v>5.31</v>
+        <v>5.11</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>11</v>
@@ -1119,10 +1111,10 @@
         <v>11</v>
       </c>
       <c r="L10" s="7">
-        <v>4.42</v>
+        <v>4.29</v>
       </c>
       <c r="M10" s="8">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -1195,10 +1187,10 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="7">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="M13" s="8">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="14">
@@ -1220,10 +1212,10 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="7">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="M14" s="7">
-        <v>0.061</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="15">
@@ -1283,7 +1275,7 @@
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="7">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="M17" s="7">
         <v>0.8</v>
@@ -1308,7 +1300,7 @@
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="7">
-        <v>1.21</v>
+        <v>1.2</v>
       </c>
       <c r="M18" s="7">
         <v>0.4</v>
@@ -1333,7 +1325,7 @@
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="7">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="M19" s="7">
         <v>0.3</v>
@@ -1396,10 +1388,10 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="7">
-        <v>3.89</v>
+        <v>3.74</v>
       </c>
       <c r="M22" s="8">
-        <v>0.024</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="23">
@@ -1421,10 +1413,10 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="7">
-        <v>3.64</v>
+        <v>3.56</v>
       </c>
       <c r="M23" s="8">
-        <v>0.028</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="24">
@@ -1484,7 +1476,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="7">
-        <v>2.61</v>
+        <v>2.59</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>11</v>
@@ -1610,7 +1602,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="7">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>11</v>
@@ -1635,10 +1627,10 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="7">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="M33" s="7">
-        <v>0.11</v>
+        <v>0.094</v>
       </c>
     </row>
     <row r="34">
@@ -1701,7 +1693,7 @@
         <v>1.6</v>
       </c>
       <c r="M36" s="8">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="37">
@@ -1726,7 +1718,7 @@
         <v>1.9</v>
       </c>
       <c r="M37" s="8">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="38">
@@ -1750,13 +1742,13 @@
       <c r="L38" s="7">
         <v>1.0</v>
       </c>
-      <c r="M38" s="7">
-        <v>0.9</v>
+      <c r="M38" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -1773,7 +1765,7 @@
     </row>
     <row r="40">
       <c r="A40" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -1794,7 +1786,7 @@
     </row>
     <row r="41">
       <c r="A41" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -1803,23 +1795,23 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="7">
-        <v>2.73</v>
+        <v>2.56</v>
       </c>
       <c r="I41" s="8">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="7">
-        <v>2.85</v>
+        <v>2.76</v>
       </c>
       <c r="M41" s="8">
-        <v>0.007</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1828,7 +1820,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="7">
-        <v>1.42</v>
+        <v>1.4</v>
       </c>
       <c r="I42" s="7">
         <v>0.2</v>
@@ -1836,15 +1828,15 @@
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="7">
-        <v>1.42</v>
+        <v>1.39</v>
       </c>
       <c r="M42" s="7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -1861,7 +1853,7 @@
     </row>
     <row r="44">
       <c r="A44" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -1882,7 +1874,7 @@
     </row>
     <row r="45">
       <c r="A45" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -1891,7 +1883,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="7">
-        <v>1.09</v>
+        <v>1.1</v>
       </c>
       <c r="I45" s="7">
         <v>0.8</v>
@@ -1899,10 +1891,10 @@
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="7">
-        <v>1.04</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>50</v>
+        <v>1.06</v>
+      </c>
+      <c r="M45" s="7">
+        <v>0.9</v>
       </c>
     </row>
     <row r="46">
@@ -1924,7 +1916,7 @@
     </row>
     <row r="47">
       <c r="A47" s="11" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -1945,7 +1937,7 @@
     </row>
     <row r="48">
       <c r="A48" s="11" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -1954,23 +1946,23 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="7">
-        <v>1.52</v>
+        <v>1.54</v>
       </c>
       <c r="I48" s="8">
-        <v>0.026</v>
+        <v>0.017</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="7">
-        <v>1.44</v>
+        <v>1.51</v>
       </c>
       <c r="M48" s="7">
-        <v>0.12</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="11" t="s">
-        <v>54</v>
+      <c r="A49" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -1978,24 +1970,16 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
-      <c r="H49" s="7">
-        <v>2.34</v>
-      </c>
-      <c r="I49" s="7">
-        <v>0.11</v>
-      </c>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
-      <c r="L49" s="7">
-        <v>3.09</v>
-      </c>
-      <c r="M49" s="7">
-        <v>0.086</v>
-      </c>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="s">
-        <v>55</v>
+      <c r="A50" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -2003,16 +1987,20 @@
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
+      <c r="H50" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
+      <c r="L50" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="M50" s="10"/>
     </row>
     <row r="51">
       <c r="A51" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -2020,20 +2008,24 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
-      <c r="H51" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="10"/>
+      <c r="H51" s="7">
+        <v>1.13</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0.6</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="10"/>
-      <c r="L51" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M51" s="10"/>
+      <c r="L51" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -2042,23 +2034,23 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="7">
-        <v>1.15</v>
+        <v>0.91</v>
       </c>
       <c r="I52" s="7">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="7">
-        <v>0.98</v>
-      </c>
-      <c r="M52" s="7" t="s">
-        <v>50</v>
+        <v>0.83</v>
+      </c>
+      <c r="M52" s="7">
+        <v>0.5</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="11" t="s">
-        <v>58</v>
+      <c r="A53" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
@@ -2066,24 +2058,16 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-      <c r="H53" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="I53" s="7">
-        <v>0.7</v>
-      </c>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
-      <c r="L53" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="M53" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="s">
-        <v>59</v>
+      <c r="A54" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -2091,11 +2075,15 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
+      <c r="H54" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
-      <c r="L54" s="10"/>
+      <c r="L54" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="M54" s="10"/>
     </row>
     <row r="55">
@@ -2108,20 +2096,24 @@
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I55" s="10"/>
+      <c r="H55" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0.4</v>
+      </c>
       <c r="J55" s="12"/>
       <c r="K55" s="10"/>
-      <c r="L55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M55" s="10"/>
+      <c r="L55" s="7">
+        <v>1.37</v>
+      </c>
+      <c r="M55" s="7">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="11" t="s">
-        <v>33</v>
+      <c r="A56" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -2129,24 +2121,16 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
-      <c r="H56" s="7">
-        <v>0.86</v>
-      </c>
-      <c r="I56" s="7">
-        <v>0.6</v>
-      </c>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
-      <c r="L56" s="7">
-        <v>0.77</v>
-      </c>
-      <c r="M56" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
     </row>
     <row r="57">
       <c r="A57" s="11" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -2154,24 +2138,20 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I57" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="H57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="12"/>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
-      <c r="L57" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="M57" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="L57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M57" s="12"/>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="s">
-        <v>61</v>
+      <c r="A58" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -2179,16 +2159,24 @@
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
+      <c r="H58" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="I58" s="7">
+        <v>0.5</v>
+      </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
+      <c r="L58" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="M58" s="7">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="11" t="s">
-        <v>34</v>
+      <c r="A59" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -2196,20 +2184,24 @@
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
-      <c r="H59" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="10"/>
+      <c r="H59" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="J59" s="12"/>
       <c r="K59" s="10"/>
-      <c r="L59" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M59" s="10"/>
+      <c r="L59" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="M59" s="8">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="11" t="s">
-        <v>62</v>
+      <c r="A60" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -2217,24 +2209,16 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
-      <c r="H60" s="7">
-        <v>0.65</v>
-      </c>
-      <c r="I60" s="7">
-        <v>0.4</v>
-      </c>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
-      <c r="L60" s="7">
-        <v>1.64</v>
-      </c>
-      <c r="M60" s="7">
-        <v>0.4</v>
-      </c>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
     </row>
     <row r="61">
       <c r="A61" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -2242,24 +2226,20 @@
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
-      <c r="H61" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="I61" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="K61" s="12"/>
-      <c r="L61" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="M61" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="L61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M61" s="12"/>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="s">
-        <v>64</v>
+      <c r="A62" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -2267,24 +2247,24 @@
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
-      <c r="H62" s="7">
-        <v>1.05</v>
-      </c>
-      <c r="I62" s="8">
-        <v>0.001</v>
-      </c>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="K62" s="7">
+        <v>0.12</v>
+      </c>
       <c r="L62" s="7">
-        <v>1.06</v>
+        <v>1.52</v>
       </c>
       <c r="M62" s="8">
-        <v>0.006</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="6" t="s">
-        <v>65</v>
+      <c r="A63" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -2294,14 +2274,22 @@
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
+      <c r="J63" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="K63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="L63" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="M63" s="7">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -2322,7 +2310,7 @@
     </row>
     <row r="65">
       <c r="A65" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -2347,7 +2335,7 @@
     </row>
     <row r="66">
       <c r="A66" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -2409,7 +2397,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -2589,10 +2577,10 @@
         <v>0.3</v>
       </c>
       <c r="H7" s="7">
-        <v>1.86</v>
+        <v>1.88</v>
       </c>
       <c r="I7" s="8">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="J7" s="7">
         <v>2.04</v>
@@ -2601,7 +2589,7 @@
         <v>0.001</v>
       </c>
       <c r="L7" s="7">
-        <v>1.32</v>
+        <v>1.35</v>
       </c>
       <c r="M7" s="7">
         <v>0.3</v>
@@ -2630,7 +2618,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="7">
-        <v>2.97</v>
+        <v>2.98</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>11</v>
@@ -2642,10 +2630,10 @@
         <v>11</v>
       </c>
       <c r="L8" s="7">
-        <v>2.04</v>
+        <v>2.06</v>
       </c>
       <c r="M8" s="8">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="9">
@@ -2671,10 +2659,10 @@
         <v>0.007</v>
       </c>
       <c r="H9" s="7">
-        <v>2.39</v>
+        <v>2.47</v>
       </c>
       <c r="I9" s="8">
-        <v>0.005</v>
+        <v>0.003</v>
       </c>
       <c r="J9" s="7">
         <v>4.09</v>
@@ -2683,10 +2671,10 @@
         <v>11</v>
       </c>
       <c r="L9" s="7">
-        <v>1.49</v>
+        <v>1.53</v>
       </c>
       <c r="M9" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10">
@@ -2712,7 +2700,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="7">
-        <v>3.24</v>
+        <v>3.26</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>11</v>
@@ -2724,10 +2712,10 @@
         <v>11</v>
       </c>
       <c r="L10" s="7">
-        <v>2.17</v>
+        <v>2.19</v>
       </c>
       <c r="M10" s="8">
-        <v>0.025</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="11">
@@ -2787,10 +2775,10 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="7">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="M13" s="7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14">
@@ -2812,10 +2800,10 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="7">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
       <c r="M14" s="7">
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15">
@@ -2875,10 +2863,10 @@
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="7">
-        <v>1.27</v>
+        <v>1.3</v>
       </c>
       <c r="M17" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18">
@@ -2988,10 +2976,10 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="7">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="M22" s="8">
-        <v>0.021</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="23">
@@ -3013,10 +3001,10 @@
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="7">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="M23" s="8">
-        <v>0.016</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="24">
@@ -3227,7 +3215,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="7">
-        <v>1.28</v>
+        <v>1.22</v>
       </c>
       <c r="M33" s="7">
         <v>0.6</v>
@@ -3290,7 +3278,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="7">
-        <v>1.26</v>
+        <v>1.28</v>
       </c>
       <c r="M36" s="7">
         <v>0.2</v>
@@ -3315,10 +3303,10 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="7">
-        <v>1.79</v>
+        <v>1.84</v>
       </c>
       <c r="M37" s="8">
-        <v>0.018</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="38">
@@ -3340,7 +3328,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="7">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="M38" s="7">
         <v>0.3</v>
@@ -3348,7 +3336,7 @@
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -3365,7 +3353,7 @@
     </row>
     <row r="40">
       <c r="A40" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -3386,7 +3374,7 @@
     </row>
     <row r="41">
       <c r="A41" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -3395,23 +3383,23 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="7">
-        <v>1.93</v>
+        <v>1.97</v>
       </c>
       <c r="I41" s="8">
-        <v>0.042</v>
+        <v>0.036</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="7">
-        <v>2.45</v>
+        <v>2.47</v>
       </c>
       <c r="M41" s="8">
-        <v>0.02</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -3428,15 +3416,15 @@
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="7">
-        <v>1.67</v>
+        <v>1.61</v>
       </c>
       <c r="M42" s="7">
-        <v>0.077</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -3453,7 +3441,7 @@
     </row>
     <row r="44">
       <c r="A44" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -3474,7 +3462,7 @@
     </row>
     <row r="45">
       <c r="A45" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -3483,7 +3471,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="7">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="I45" s="7">
         <v>0.8</v>
@@ -3491,10 +3479,10 @@
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="7">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
       <c r="M45" s="7">
-        <v>0.08</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="46">
@@ -3516,7 +3504,7 @@
     </row>
     <row r="47">
       <c r="A47" s="11" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -3537,7 +3525,7 @@
     </row>
     <row r="48">
       <c r="A48" s="11" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -3546,23 +3534,23 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="7">
-        <v>1.54</v>
+        <v>1.46</v>
       </c>
       <c r="I48" s="8">
-        <v>0.017</v>
+        <v>0.033</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="7">
-        <v>1.59</v>
-      </c>
-      <c r="M48" s="8">
-        <v>0.039</v>
+        <v>1.49</v>
+      </c>
+      <c r="M48" s="7">
+        <v>0.071</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="11" t="s">
-        <v>54</v>
+      <c r="A49" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -3570,24 +3558,16 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
-      <c r="H49" s="7">
-        <v>0.48</v>
-      </c>
-      <c r="I49" s="7">
-        <v>0.4</v>
-      </c>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
-      <c r="L49" s="7">
-        <v>0.34</v>
-      </c>
-      <c r="M49" s="7">
-        <v>0.3</v>
-      </c>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="s">
-        <v>55</v>
+      <c r="A50" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -3595,16 +3575,20 @@
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
+      <c r="H50" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
+      <c r="L50" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="M50" s="10"/>
     </row>
     <row r="51">
       <c r="A51" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -3612,20 +3596,24 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
-      <c r="H51" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="10"/>
+      <c r="H51" s="7">
+        <v>0.88</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0.6</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="10"/>
-      <c r="L51" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M51" s="10"/>
+      <c r="L51" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="M51" s="7">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -3634,23 +3622,23 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="7">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="I52" s="7">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="7">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
       <c r="M52" s="7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="11" t="s">
-        <v>58</v>
+      <c r="A53" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
@@ -3658,24 +3646,16 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-      <c r="H53" s="7">
-        <v>0.87</v>
-      </c>
-      <c r="I53" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
-      <c r="L53" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="M53" s="7">
-        <v>0.3</v>
-      </c>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="s">
-        <v>59</v>
+      <c r="A54" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -3683,11 +3663,15 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
+      <c r="H54" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
-      <c r="L54" s="10"/>
+      <c r="L54" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="M54" s="10"/>
     </row>
     <row r="55">
@@ -3700,20 +3684,24 @@
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
-      <c r="H55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I55" s="10"/>
+      <c r="H55" s="7">
+        <v>1.16</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0.5</v>
+      </c>
       <c r="J55" s="12"/>
       <c r="K55" s="10"/>
-      <c r="L55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M55" s="10"/>
+      <c r="L55" s="7">
+        <v>1.16</v>
+      </c>
+      <c r="M55" s="7">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="11" t="s">
-        <v>33</v>
+      <c r="A56" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -3721,24 +3709,16 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
-      <c r="H56" s="7">
-        <v>0.96</v>
-      </c>
-      <c r="I56" s="7">
-        <v>0.9</v>
-      </c>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
-      <c r="L56" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="M56" s="7">
-        <v>0.8</v>
-      </c>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
     </row>
     <row r="57">
       <c r="A57" s="11" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -3746,24 +3726,20 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="7">
-        <v>0.22</v>
-      </c>
-      <c r="I57" s="7">
-        <v>0.2</v>
-      </c>
+      <c r="H57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="12"/>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
-      <c r="L57" s="7">
-        <v>0.38</v>
-      </c>
-      <c r="M57" s="7">
-        <v>0.4</v>
-      </c>
+      <c r="L57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M57" s="12"/>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="s">
-        <v>61</v>
+      <c r="A58" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -3771,16 +3747,24 @@
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
+      <c r="H58" s="7">
+        <v>0.47</v>
+      </c>
+      <c r="I58" s="7">
+        <v>0.072</v>
+      </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
+      <c r="L58" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="M58" s="7">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="11" t="s">
-        <v>34</v>
+      <c r="A59" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -3788,20 +3772,24 @@
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
-      <c r="H59" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="10"/>
+      <c r="H59" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="J59" s="12"/>
       <c r="K59" s="10"/>
-      <c r="L59" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M59" s="10"/>
+      <c r="L59" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="M59" s="8">
+        <v>0.007</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="11" t="s">
-        <v>62</v>
+      <c r="A60" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -3809,24 +3797,16 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
-      <c r="H60" s="7">
-        <v>0.46</v>
-      </c>
-      <c r="I60" s="7">
-        <v>0.07</v>
-      </c>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
-      <c r="L60" s="7">
-        <v>0.44</v>
-      </c>
-      <c r="M60" s="7">
-        <v>0.14</v>
-      </c>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
     </row>
     <row r="61">
       <c r="A61" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -3834,24 +3814,20 @@
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
-      <c r="H61" s="7">
-        <v>3.72</v>
-      </c>
-      <c r="I61" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="J61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="K61" s="12"/>
-      <c r="L61" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="M61" s="7">
-        <v>0.4</v>
-      </c>
+      <c r="L61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M61" s="12"/>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="s">
-        <v>64</v>
+      <c r="A62" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -3859,24 +3835,24 @@
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
-      <c r="H62" s="7">
-        <v>1.06</v>
-      </c>
-      <c r="I62" s="8">
-        <v>0.001</v>
-      </c>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="K62" s="7">
+        <v>0.15</v>
+      </c>
       <c r="L62" s="7">
-        <v>1.05</v>
-      </c>
-      <c r="M62" s="8">
-        <v>0.008</v>
+        <v>1.07</v>
+      </c>
+      <c r="M62" s="7">
+        <v>0.7</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="6" t="s">
-        <v>65</v>
+      <c r="A63" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -3886,14 +3862,22 @@
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
+      <c r="J63" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="K63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="L63" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="M63" s="7">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -3914,7 +3898,7 @@
     </row>
     <row r="65">
       <c r="A65" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -3939,7 +3923,7 @@
     </row>
     <row r="66">
       <c r="A66" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -3987,7 +3971,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.25"/>
-    <col customWidth="1" min="2" max="2" width="94.25"/>
+    <col customWidth="1" min="2" max="2" width="96.88"/>
     <col customWidth="1" min="3" max="3" width="92.13"/>
   </cols>
   <sheetData>
@@ -3996,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -4004,10 +3988,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -4015,10 +3999,10 @@
         <v>23</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -4026,10 +4010,10 @@
         <v>28</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -4037,10 +4021,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6">
@@ -4048,10 +4032,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
@@ -4059,10 +4043,10 @@
         <v>36</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
@@ -4070,10 +4054,10 @@
         <v>38</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
@@ -4081,32 +4065,32 @@
         <v>42</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
@@ -4114,65 +4098,65 @@
         <v>51</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4230,19 +4214,19 @@
     </row>
     <row r="2">
       <c r="A2" s="19" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
@@ -4270,19 +4254,19 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B3" s="22">
-        <v>0.2008193</v>
+        <v>0.1651608</v>
       </c>
       <c r="C3" s="22">
-        <v>0.1294163</v>
+        <v>0.1097067</v>
       </c>
       <c r="D3" s="22">
-        <v>1620.106</v>
+        <v>1472.3317</v>
       </c>
       <c r="E3" s="22">
-        <v>1653.286</v>
+        <v>1505.785</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -4310,19 +4294,19 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B4" s="22">
-        <v>0.2114602</v>
+        <v>0.1899716</v>
       </c>
       <c r="C4" s="22">
-        <v>0.1296329</v>
+        <v>0.1198587</v>
       </c>
       <c r="D4" s="22">
-        <v>1619.703</v>
+        <v>1455.5426</v>
       </c>
       <c r="E4" s="22">
-        <v>1691.585</v>
+        <v>1528.005</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
@@ -4350,19 +4334,19 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B5" s="22">
-        <v>0.4021059</v>
+        <v>0.3971459</v>
       </c>
       <c r="C5" s="22">
-        <v>0.2795054</v>
+        <v>0.2879893</v>
       </c>
       <c r="D5" s="22">
-        <v>1340.799</v>
+        <v>1177.495</v>
       </c>
       <c r="E5" s="22">
-        <v>1409.484</v>
+        <v>1247.559</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -4390,19 +4374,19 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B6" s="22">
-        <v>0.4095542</v>
+        <v>0.4470886</v>
       </c>
       <c r="C6" s="22">
-        <v>0.2804675</v>
+        <v>0.3299582</v>
       </c>
       <c r="D6" s="22">
-        <v>1339.008</v>
+        <v>1108.0885</v>
       </c>
       <c r="E6" s="22">
-        <v>1435.306</v>
+        <v>1188.727</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -4430,19 +4414,19 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B7" s="22">
-        <v>0.2041336</v>
+        <v>0.1694883</v>
       </c>
       <c r="C7" s="22">
-        <v>0.1296711</v>
+        <v>0.1105141</v>
       </c>
       <c r="D7" s="22">
-        <v>1619.632</v>
+        <v>1470.9964</v>
       </c>
       <c r="E7" s="22">
-        <v>1663.846</v>
+        <v>1515.597</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -4473,16 +4457,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="22">
-        <v>0.5587417</v>
+        <v>0.5947864</v>
       </c>
       <c r="C8" s="22">
-        <v>0.3994219</v>
+        <v>0.4525958</v>
       </c>
       <c r="D8" s="22">
-        <v>1117.641</v>
+        <v>905.2753</v>
       </c>
       <c r="E8" s="22">
-        <v>1291.654</v>
+        <v>1066.349</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -4540,7 +4524,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -4567,20 +4551,20 @@
       <c r="AB10" s="18"/>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>95</v>
+      <c r="A11" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -4607,19 +4591,19 @@
       <c r="AB11" s="18"/>
     </row>
     <row r="12">
-      <c r="A12" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="22">
+      <c r="A12" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="27">
         <v>0.2008193</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="27">
         <v>0.1294163</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="27">
         <v>1620.106</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="27">
         <v>1653.286</v>
       </c>
       <c r="F12" s="18"/>
@@ -4647,19 +4631,19 @@
       <c r="AB12" s="18"/>
     </row>
     <row r="13">
-      <c r="A13" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="22">
+      <c r="A13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="27">
         <v>0.2114602</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="27">
         <v>0.1296329</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="27">
         <v>1619.703</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="27">
         <v>1691.585</v>
       </c>
       <c r="F13" s="18"/>
@@ -4687,19 +4671,19 @@
       <c r="AB13" s="18"/>
     </row>
     <row r="14">
-      <c r="A14" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="22">
+      <c r="A14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="27">
         <v>0.4021059</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="27">
         <v>0.2795054</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="27">
         <v>1340.799</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="27">
         <v>1409.484</v>
       </c>
       <c r="F14" s="18"/>
@@ -4727,20 +4711,20 @@
       <c r="AB14" s="18"/>
     </row>
     <row r="15">
-      <c r="A15" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="22">
-        <v>0.4095542</v>
-      </c>
-      <c r="C15" s="22">
-        <v>0.2804675</v>
-      </c>
-      <c r="D15" s="22">
-        <v>1339.008</v>
-      </c>
-      <c r="E15" s="22">
-        <v>1435.306</v>
+      <c r="A15" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="27">
+        <v>0.405813</v>
+      </c>
+      <c r="C15" s="27">
+        <v>0.2805043</v>
+      </c>
+      <c r="D15" s="27">
+        <v>1338.94</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1419.188</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
@@ -4767,19 +4751,19 @@
       <c r="AB15" s="18"/>
     </row>
     <row r="16">
-      <c r="A16" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="22">
+      <c r="A16" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="27">
         <v>0.2041336</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="27">
         <v>0.1296711</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="27">
         <v>1619.632</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="27">
         <v>1663.846</v>
       </c>
       <c r="F16" s="18"/>
@@ -4807,20 +4791,20 @@
       <c r="AB16" s="18"/>
     </row>
     <row r="17">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="22">
-        <v>0.5587417</v>
-      </c>
-      <c r="C17" s="22">
-        <v>0.3994219</v>
-      </c>
-      <c r="D17" s="22">
-        <v>1117.641</v>
-      </c>
-      <c r="E17" s="22">
-        <v>1291.654</v>
+      <c r="B17" s="27">
+        <v>0.5563482</v>
+      </c>
+      <c r="C17" s="27">
+        <v>0.4003092</v>
+      </c>
+      <c r="D17" s="27">
+        <v>1115.99</v>
+      </c>
+      <c r="E17" s="27">
+        <v>1274.649</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -4847,7 +4831,7 @@
       <c r="AB17" s="18"/>
     </row>
     <row r="18">
-      <c r="A18" s="18"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>

</xml_diff>